<commit_message>
email en cci 2
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>L6</t>
+  </si>
+  <si>
+    <t>1a25a65c-c794-4313-ac4d-6c43c8ef732f</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
@@ -671,6 +674,32 @@
         <v>22</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
update dto et pupeteer sur vps
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -107,6 +107,24 @@
   </si>
   <si>
     <t>1a25a65c-c794-4313-ac4d-6c43c8ef732f</t>
+  </si>
+  <si>
+    <t>539b9bf3-0642-4945-a00e-31319c9cb371</t>
+  </si>
+  <si>
+    <t>2025-09-28T00:00:00.000Z</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>transchool</t>
+  </si>
+  <si>
+    <t>3e7cfffc-744c-4772-9898-c2a2e7dcefea</t>
+  </si>
+  <si>
+    <t>T2</t>
   </si>
 </sst>
 </file>
@@ -483,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
@@ -700,6 +718,64 @@
         <v>22</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
mise a jour du nom dans objet mail
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -239,6 +239,60 @@
   </si>
   <si>
     <t>Doit vraiment passer un coup de balai et de serpière</t>
+  </si>
+  <si>
+    <t>23/11/2025</t>
+  </si>
+  <si>
+    <t>15:33</t>
+  </si>
+  <si>
+    <t>Saint-avold</t>
+  </si>
+  <si>
+    <t>Jean jacque</t>
+  </si>
+  <si>
+    <t>Poteau arrêt</t>
+  </si>
+  <si>
+    <t>casas</t>
+  </si>
+  <si>
+    <t>transchool</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>15:44</t>
+  </si>
+  <si>
+    <t>carling</t>
+  </si>
+  <si>
+    <t>LORANG</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>24/11/2025</t>
+  </si>
+  <si>
+    <t>06:49</t>
+  </si>
+  <si>
+    <t>06:01</t>
+  </si>
+  <si>
+    <t>Merlebach</t>
+  </si>
+  <si>
+    <t>Friderich</t>
+  </si>
+  <si>
+    <t>SA24</t>
   </si>
 </sst>
 </file>
@@ -615,7 +669,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -1084,6 +1138,303 @@
         <v>58</v>
       </c>
     </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W5" t="s">
+        <v>83</v>
+      </c>
+      <c r="X5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y5">
+        <v>19963</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP5">
+        <v>15</v>
+      </c>
+      <c r="AQ5">
+        <v>3</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6" t="s">
+        <v>82</v>
+      </c>
+      <c r="W6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y6">
+        <v>25825</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP6">
+        <v>20</v>
+      </c>
+      <c r="AQ6">
+        <v>3</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" t="s">
+        <v>64</v>
+      </c>
+      <c r="T7" t="s">
+        <v>93</v>
+      </c>
+      <c r="X7" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y7">
+        <v>22320</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP7">
+        <v>10</v>
+      </c>
+      <c r="AQ7">
+        <v>2</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
retour a prisma 6
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="118">
   <si>
     <t>Date</t>
   </si>
@@ -293,6 +293,78 @@
   </si>
   <si>
     <t>SA24</t>
+  </si>
+  <si>
+    <t>16:18</t>
+  </si>
+  <si>
+    <t>16:17</t>
+  </si>
+  <si>
+    <t>l'hopital</t>
+  </si>
+  <si>
+    <t>bossand</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>16:23</t>
+  </si>
+  <si>
+    <t>16:22</t>
+  </si>
+  <si>
+    <t>poli</t>
+  </si>
+  <si>
+    <t>casc</t>
+  </si>
+  <si>
+    <t>PT01</t>
+  </si>
+  <si>
+    <t>16:30</t>
+  </si>
+  <si>
+    <t>16:26</t>
+  </si>
+  <si>
+    <t>momerstroff</t>
+  </si>
+  <si>
+    <t>Lr</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>18:10</t>
+  </si>
+  <si>
+    <t>18:08</t>
+  </si>
+  <si>
+    <t>18:44</t>
+  </si>
+  <si>
+    <t>18:43</t>
+  </si>
+  <si>
+    <t>Rosbruck</t>
+  </si>
+  <si>
+    <t>chahid</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>19:10</t>
+  </si>
+  <si>
+    <t>19:09</t>
   </si>
 </sst>
 </file>
@@ -669,7 +741,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR7"/>
+  <dimension ref="A1:AR13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -1435,6 +1507,570 @@
         <v>58</v>
       </c>
     </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" t="s">
+        <v>82</v>
+      </c>
+      <c r="W8" t="s">
+        <v>98</v>
+      </c>
+      <c r="X8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y8">
+        <v>22635</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP8">
+        <v>32</v>
+      </c>
+      <c r="AQ8">
+        <v>2</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" t="s">
+        <v>63</v>
+      </c>
+      <c r="L9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R9" t="s">
+        <v>103</v>
+      </c>
+      <c r="X9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y9">
+        <v>20325</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP9">
+        <v>10</v>
+      </c>
+      <c r="AQ9">
+        <v>2</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10" t="s">
+        <v>107</v>
+      </c>
+      <c r="S10" t="s">
+        <v>108</v>
+      </c>
+      <c r="X10" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y10">
+        <v>22320</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP10">
+        <v>20</v>
+      </c>
+      <c r="AQ10">
+        <v>1</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" t="s">
+        <v>72</v>
+      </c>
+      <c r="X11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y11">
+        <v>22325</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP11">
+        <v>10</v>
+      </c>
+      <c r="AQ11">
+        <v>1</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" t="s">
+        <v>107</v>
+      </c>
+      <c r="S12" t="s">
+        <v>115</v>
+      </c>
+      <c r="X12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y12">
+        <v>19965</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP12">
+        <v>32</v>
+      </c>
+      <c r="AQ12">
+        <v>1</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" t="s">
+        <v>63</v>
+      </c>
+      <c r="L13" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T13" t="s">
+        <v>65</v>
+      </c>
+      <c r="X13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y13">
+        <v>22352</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP13">
+        <v>10</v>
+      </c>
+      <c r="AQ13">
+        <v>2</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
rectification dto pour numLignHH
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="124">
   <si>
     <t>Date</t>
   </si>
@@ -365,6 +365,24 @@
   </si>
   <si>
     <t>19:09</t>
+  </si>
+  <si>
+    <t>25/11/2025</t>
+  </si>
+  <si>
+    <t>19:18</t>
+  </si>
+  <si>
+    <t>18:18</t>
+  </si>
+  <si>
+    <t>hombourgHaut</t>
+  </si>
+  <si>
+    <t>pluvieux</t>
+  </si>
+  <si>
+    <t>BANGOURA</t>
   </si>
 </sst>
 </file>
@@ -741,7 +759,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR13"/>
+  <dimension ref="A1:AR14"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -2071,6 +2089,95 @@
         <v>58</v>
       </c>
     </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" t="s">
+        <v>121</v>
+      </c>
+      <c r="X14" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y14">
+        <v>22320</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP14">
+        <v>10</v>
+      </c>
+      <c r="AQ14">
+        <v>1</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
mise a jour bdd niveau sécurité
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B06C6A-647D-4F8E-A808-0196454092E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
-    <sheet name="Controles" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Controles" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -149,28 +148,58 @@
     <t>Nom Contrôleur</t>
   </si>
   <si>
+    <t>24/11/2025</t>
+  </si>
+  <si>
+    <t>07:32</t>
+  </si>
+  <si>
+    <t>07:25</t>
+  </si>
+  <si>
+    <t>Saint-Avold</t>
+  </si>
+  <si>
+    <t>FRIDERICH</t>
+  </si>
+  <si>
+    <t>Conforme</t>
+  </si>
+  <si>
+    <t>Poteau arrêt</t>
+  </si>
+  <si>
+    <t>Ras</t>
+  </si>
+  <si>
+    <t>rgeFluo57</t>
+  </si>
+  <si>
+    <t>Sa</t>
+  </si>
+  <si>
+    <t>SA24</t>
+  </si>
+  <si>
+    <t>beau</t>
+  </si>
+  <si>
+    <t>Non conforme</t>
+  </si>
+  <si>
+    <t>Propre</t>
+  </si>
+  <si>
     <t>Non observable</t>
   </si>
   <si>
-    <t>rgeFluo57</t>
-  </si>
-  <si>
-    <t>beau</t>
-  </si>
-  <si>
-    <t>Conforme</t>
-  </si>
-  <si>
-    <t>Propre</t>
-  </si>
-  <si>
-    <t>Sa</t>
-  </si>
-  <si>
-    <t>Non conforme</t>
-  </si>
-  <si>
-    <t>Poteau arrêt</t>
+    <t>BANGOURA</t>
+  </si>
+  <si>
+    <t>07:50</t>
+  </si>
+  <si>
+    <t>Hopital</t>
   </si>
   <si>
     <t>casas</t>
@@ -179,50 +208,53 @@
     <t>transchool</t>
   </si>
   <si>
-    <t>24/11/2025</t>
-  </si>
-  <si>
-    <t>SA24</t>
-  </si>
-  <si>
-    <t>07:32</t>
-  </si>
-  <si>
-    <t>07:25</t>
-  </si>
-  <si>
-    <t>Saint-Avold</t>
-  </si>
-  <si>
-    <t>FRIDERICH</t>
-  </si>
-  <si>
-    <t>Ras</t>
-  </si>
-  <si>
-    <t>BANGOURA</t>
-  </si>
-  <si>
-    <t>07:50</t>
-  </si>
-  <si>
-    <t>Hopital</t>
-  </si>
-  <si>
     <t>T3</t>
+  </si>
+  <si>
+    <t>19/01/2026</t>
+  </si>
+  <si>
+    <t>13:55</t>
+  </si>
+  <si>
+    <t>poli</t>
+  </si>
+  <si>
+    <t>Bangoura</t>
+  </si>
+  <si>
+    <t>tufd</t>
+  </si>
+  <si>
+    <t>ras</t>
+  </si>
+  <si>
+    <t>14:07</t>
+  </si>
+  <si>
+    <t>14:05</t>
+  </si>
+  <si>
+    <t>Abris bus</t>
+  </si>
+  <si>
+    <t>RAS</t>
+  </si>
+  <si>
+    <t>forbus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -585,14 +617,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AR5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="3" width="12" customWidth="1"/>
@@ -759,100 +791,100 @@
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="X2" t="s">
         <v>55</v>
-      </c>
-      <c r="X2" t="s">
-        <v>46</v>
       </c>
       <c r="Y2">
         <v>21831</v>
       </c>
       <c r="Z2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AA2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AB2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AC2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AD2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="AE2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AF2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AG2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="AH2" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="AI2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AJ2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AK2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AL2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AM2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AN2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AO2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="AP2">
         <v>26</v>
@@ -861,93 +893,93 @@
         <v>1</v>
       </c>
       <c r="AR2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" t="s">
         <v>62</v>
       </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="M3" t="s">
         <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" t="s">
-        <v>53</v>
       </c>
       <c r="W3" t="s">
         <v>64</v>
       </c>
       <c r="X3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="Y3">
         <v>21831</v>
       </c>
       <c r="Z3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AA3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AB3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AC3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AD3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="AE3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AF3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AG3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="AH3" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="AI3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AJ3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AK3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AL3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AM3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AN3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AO3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="AP3">
         <v>56</v>
@@ -956,11 +988,207 @@
         <v>0</v>
       </c>
       <c r="AR3" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" t="s">
+        <v>54</v>
+      </c>
+      <c r="X4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4">
+        <v>10235</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP4">
+        <v>4</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" t="s">
+        <v>75</v>
+      </c>
+      <c r="X5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y5">
+        <v>100125</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP5">
+        <v>30</v>
+      </c>
+      <c r="AQ5">
+        <v>1</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mise a jour des packages
</commit_message>
<xml_diff>
--- a/controle/controle.xlsx
+++ b/controle/controle.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -242,6 +242,21 @@
   </si>
   <si>
     <t>forbus</t>
+  </si>
+  <si>
+    <t>15:31</t>
+  </si>
+  <si>
+    <t>15:30</t>
+  </si>
+  <si>
+    <t>casc</t>
+  </si>
+  <si>
+    <t>Lr</t>
+  </si>
+  <si>
+    <t>125</t>
   </si>
 </sst>
 </file>
@@ -618,7 +633,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR5"/>
+  <dimension ref="A1:AR6"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="F18" sqref="F18"/>
@@ -1187,6 +1202,113 @@
         <v>59</v>
       </c>
     </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6" t="s">
+        <v>79</v>
+      </c>
+      <c r="P6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y6">
+        <v>102563</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP6">
+        <v>10</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>